<commit_message>
rapport + journal de travail
</commit_message>
<xml_diff>
--- a/doc/Journal/Journal.xlsx
+++ b/doc/Journal/Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>DATE</t>
   </si>
@@ -72,6 +72,42 @@
   </si>
   <si>
     <t>Ajout entrée analogique pour capteur de pression, màj du schèma et présentation de l'étude.</t>
+  </si>
+  <si>
+    <t>Vacances</t>
+  </si>
+  <si>
+    <t>Montage</t>
+  </si>
+  <si>
+    <t>Montage et tests</t>
+  </si>
+  <si>
+    <t>Programmation firmware</t>
+  </si>
+  <si>
+    <t>Centrale inertiell BNO055</t>
+  </si>
+  <si>
+    <t>Carte SD</t>
+  </si>
+  <si>
+    <t>Tests et lectures</t>
+  </si>
+  <si>
+    <t>Design mécanique et tests</t>
+  </si>
+  <si>
+    <t>Implémentation capteur de pression</t>
+  </si>
+  <si>
+    <t>ADC - Capteur de pression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmation firmware </t>
+  </si>
+  <si>
+    <t>Gestion des temps processeur</t>
   </si>
 </sst>
 </file>
@@ -431,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.85546875" defaultRowHeight="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -577,6 +613,161 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>44972</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>44979</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>44986</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>44993</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>45000</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45007</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>45014</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>45021</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>45028</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>45035</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>45042</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>45049</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>45056</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>45063</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>45070</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>45077</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>